<commit_message>
Add files results and modify order ranking
</commit_message>
<xml_diff>
--- a/results/Resultados-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS.xlsx
+++ b/results/Resultados-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS.xlsx
@@ -63,14 +63,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="44.3046875" customWidth="true"/>
-    <col min="2" max="2" width="38.859375" customWidth="true"/>
+    <col min="2" max="2" width="39.03515625" customWidth="true"/>
     <col min="3" max="3" width="63.49609375" customWidth="true"/>
     <col min="4" max="4" width="23.171875" customWidth="true"/>
     <col min="5" max="5" width="23.18359375" customWidth="true"/>
@@ -116,10 +116,10 @@
         <v>368.4868441</v>
       </c>
       <c r="D2" t="n">
-        <v>22.0</v>
+        <v>35.0</v>
       </c>
       <c r="E2" t="n">
-        <v>42.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="3">
@@ -233,7 +233,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ARAUJO MENDOZA JEFFERSON ANDRES</t>
+          <t>PARRAGA TAIPE ARIANA BETZABET</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -242,7 +242,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>274.4517617</v>
+        <v>294.956147</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -256,7 +256,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ALDANA COTRINA NANCY CRISTINA</t>
+          <t>ATAHUA RIVERA DENNIS RICARDO</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -265,7 +265,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>256.72149555</v>
+        <v>287.22588085</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -279,7 +279,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ORCASITAS GARCIA SHEILA PAOLA</t>
+          <t>ARAUJO MENDOZA JEFFERSON ANDRES</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -288,7 +288,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>253.9473764</v>
+        <v>274.4517617</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -302,7 +302,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ESQUIVEL YGNACIO ZENAYDA</t>
+          <t>ALDANA COTRINA NANCY CRISTINA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -311,7 +311,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>234.4517617</v>
+        <v>256.72149555</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -325,7 +325,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CHIRA SIANCAS JOSE ANTHONY</t>
+          <t>ENRRIQUEZ TTUPA ANTONELA SILVANA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -334,7 +334,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>233.4429911</v>
+        <v>254.19956905</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -348,7 +348,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RAMOS ARTEAGA SANTIAGO OBED</t>
+          <t>ORCASITAS GARCIA SHEILA PAOLA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -357,7 +357,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>224.4517617</v>
+        <v>253.9473764</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -371,7 +371,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ALVAREZ RAMIREZ IVAN LEONARDO</t>
+          <t>GOMEZ BASTIDAS CELIA JUANA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -380,7 +380,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>223.19079845</v>
+        <v>243.69518375</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -394,7 +394,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ORTEGA RIVADENEYRA NICOLE KIARA</t>
+          <t>ESQUIVEL YGNACIO ZENAYDA</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -403,7 +403,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>217.73026615</v>
+        <v>234.4517617</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -417,7 +417,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>GOMEZ ORTIZ HAJIME GABRIEL</t>
+          <t>CHIRA SIANCAS JOSE ANTHONY</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -426,7 +426,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>213.19079845</v>
+        <v>233.4429911</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -440,7 +440,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ALARCON CUADROS ANGELICA ELIZABETH</t>
+          <t>RAMOS ARTEAGA SANTIAGO OBED</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -449,7 +449,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>203.9473764</v>
+        <v>224.4517617</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -463,7 +463,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ARIAS VIZCARRA NAHOMI GERALDINE</t>
+          <t>ALVAREZ RAMIREZ IVAN LEONARDO</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>202.68641315</v>
+        <v>223.19079845</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -486,7 +486,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>GODOY CUCHO NICOLE CAROLINE</t>
+          <t>LOCONI PEREZ MACARENA GABRIELA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>192.4342205</v>
+        <v>223.19079845</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ROCA ALVAREZ MIRIAN JAKELIN</t>
+          <t>ORTEGA RIVADENEYRA NICOLE KIARA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>186.21711025</v>
+        <v>217.73026615</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LAURA CAMPOS JUAN SEBASTIAN</t>
+          <t>POLO ESTEBAN SANDRITA LIZETH</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>182.4342205</v>
+        <v>215.9649176</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -555,7 +555,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LOPEZ VASQUEZ BRUNO ANDREE</t>
+          <t>GOMEZ ORTIZ HAJIME GABRIEL</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>182.18202785</v>
+        <v>213.19079845</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MATEO MATEO VANESSA</t>
+          <t>VALENZUELA VALVERDE ANELL JAZMIN</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>171.92983521</v>
+        <v>213.19079845</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ESPONDA PALMA MARCIA SOFIA</t>
+          <t>COLLANTES GONZALES ALHELY MILAGROS</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>171.92983521</v>
+        <v>207.9824588</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -624,7 +624,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ARIAS RAMIREZ JANIS MILAGROS</t>
+          <t>FERNANDEZ VARGAS DOLLY NADIA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>171.92983521</v>
+        <v>206.21711025</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -647,7 +647,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BENITES CABELLO FATIMA CAROLINE</t>
+          <t>ALARCON CUADROS ANGELICA ELIZABETH</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>171.92983521</v>
+        <v>203.9473764</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -670,7 +670,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>PILLACA CAMPOS VALERIA MERCEDES</t>
+          <t>ARIAS VIZCARRA NAHOMI GERALDINE</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -679,11 +679,11 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>171.9298352</v>
+        <v>202.68641315</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MERINO LUGO SANDRA BRIYIT</t>
+          <t>CARDENAS VILLAGARAY EDISON WILVER</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -702,11 +702,11 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>163.4429911</v>
+        <v>192.4342205</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CRUZ PILLACA MELISA</t>
+          <t>DE LA CRUZ LOPEZ MASSIEL VICTORIA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -725,11 +725,11 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>161.9298352</v>
+        <v>192.4342205</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -739,7 +739,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ESPINOZA VALENCIAS ANGEL MANUEL</t>
+          <t>GODOY CUCHO NICOLE CAROLINE</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -748,11 +748,11 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>153.19079845</v>
+        <v>192.4342205</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CAMPOS PACHECO MATHEW YAGO</t>
+          <t>ROCA ALVAREZ MIRIAN JAKELIN</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -771,11 +771,11 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>146.9736882</v>
+        <v>186.21711025</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>LIZARRAGA ISUIZA ASTRID YANIRA</t>
+          <t>LAURA CAMPOS JUAN SEBASTIAN</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -794,11 +794,11 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>141.67764255</v>
+        <v>182.4342205</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ZAVALETA HERRERA MADELEYNE BRIGHITE</t>
+          <t>DE LA CRUZ LAURA CAROLAY JADE</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -817,11 +817,11 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>132.18202785</v>
+        <v>182.18202785</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ARANIBAR MERCADO XIOMARA JAZMIN</t>
+          <t>LOPEZ VASQUEZ BRUNO ANDREE</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -840,11 +840,11 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>131.67764255</v>
+        <v>182.18202785</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ESPINOZA LAYME EVELYN HAYDEE</t>
+          <t>ALVARADO PRADO KETTY PAOLA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -863,11 +863,11 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>130.9210646</v>
+        <v>173.19079845</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PAIMA CHAVARRI RENZO GABRIEL</t>
+          <t>ARIAS RAMIREZ JANIS MILAGROS</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -886,11 +886,11 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>130.9210646</v>
+        <v>171.92983521</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CHAVEZ LAGUNA MARIA FERNANDA</t>
+          <t>BENITES CABELLO FATIMA CAROLINE</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -909,11 +909,11 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>130.9210646</v>
+        <v>171.92983521</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>HUAMANQUISPE CHIPAO SOLIMAR</t>
+          <t>ESPONDA PALMA MARCIA SOFIA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -932,11 +932,11 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>130.9210646</v>
+        <v>171.92983521</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>FLORES CLEMENTE FOLLY NAHIROBY</t>
+          <t>MATEO MATEO VANESSA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -955,11 +955,11 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>120.66887195</v>
+        <v>171.92983521</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>NO INGRESO</t>
+          <t>INGRESO</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>YARLEQUE LITANO GABRIEL ANGEL</t>
+          <t>PILLACA CAMPOS VALERIA MERCEDES</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>120.66887195</v>
+        <v>171.9298352</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -992,7 +992,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SALINAS RAMOS MELODI EDITH</t>
+          <t>MARCALAYA GUIZADO ARELLYS VALERIA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>111.67764255</v>
+        <v>163.4429911</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>RAMOS GONZALES KELIN SOFIA</t>
+          <t>MERINO LUGO SANDRA BRIYIT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>110.4166793</v>
+        <v>163.4429911</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>QUICAÑA HUAMAN NAYELY LUCERO</t>
+          <t>CRUZ PILLACA MELISA</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>100.16448665</v>
+        <v>161.9298352</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>MURO MIRANDA BRENDA VIVIAN</t>
+          <t>ESPINOZA VALENCIAS ANGEL MANUEL</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>83.9473764</v>
+        <v>153.19079845</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DAVILA CHAVEZ ALISSON DAYANA</t>
+          <t>DE LA TORRE TEJEDA DANIELA ALEJANDRA</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>80.9210646</v>
+        <v>152.9386058</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1107,20 +1107,549 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>TELLO RUIZ GUADALUPE LIZETH</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>151.4254499</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>CAMPOS PACHECO MATHEW YAGO</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>146.9736882</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ATAHUALPA DAVILA VALERIA ABIGAIL</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>146.21711025</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>LIZARRAGA ISUIZA ASTRID YANIRA</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>141.67764255</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>JIMENEZ CASTILLO HEIDI JUDITH</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>141.17325725</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SABINO VENANCIO NITZY LUISANA</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>141.17325725</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CALAPUJA CHURA ANTHONY</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>135.9649176</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ZAVALETA HERRERA MADELEYNE BRIGHITE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>132.18202785</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ARANIBAR MERCADO XIOMARA JAZMIN</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>131.67764255</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>CHAVEZ LAGUNA MARIA FERNANDA</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>130.9210646</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>CHUMPITAZ ESPINOZA CINTHYA GIANNINA</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>130.9210646</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ESPINOZA LAYME EVELYN HAYDEE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>130.9210646</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HUAMANQUISPE CHIPAO SOLIMAR</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>130.9210646</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>PAIMA CHAVARRI RENZO GABRIEL</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>130.9210646</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>FLORES CLEMENTE FOLLY NAHIROBY</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>120.66887195</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>TELLO HUAMANYAURI LUIS MIGUEL</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>120.66887195</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>YARLEQUE LITANO GABRIEL ANGEL</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>120.66887195</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>SALINAS RAMOS MELODI EDITH</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>111.67764255</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>RAMOS GONZALES KELIN SOFIA</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>110.4166793</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>QUICAÑA HUAMAN NAYELY LUCERO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>100.16448665</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>MURO MIRANDA BRENDA VIVIAN</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>83.9473764</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DAVILA CHAVEZ ALISSON DAYANA</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>80.9210646</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>GOMEZ VELA MARISA BRIGITH</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
         <v>69.4079087</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>NO INGRESO</t>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>NO INGRESO</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>BONETT HUAMAN LESLY PATRICIA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>EXAMEN ORDINARIO-EDUCACIÓN SECUNDARIA ESPECIALIDAD: INGLÉS</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>AUSENTE</t>
         </is>
       </c>
     </row>

</xml_diff>